<commit_message>
Add acrylic buffer design
Add SVG file for laser cutting acrylic buffer layer
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debra\Dropbox\Documents\GitHub\ArticulatedPCBs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEAF8DE-04E1-4AB9-9FA9-2C11E7043242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6366BF-A554-476C-8DA5-CCE7B0DC6D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10515" yWindow="3000" windowWidth="16695" windowHeight="13335" xr2:uid="{421486F9-22EC-4FE7-B292-C13435E23E73}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>PCB Components</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>DF23C-10DS-0.5V(51)</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>1/16" (1.6mm) acrylic for laser-cut buffer layer</t>
+  </si>
+  <si>
+    <t>1 buffer per link</t>
   </si>
 </sst>
 </file>
@@ -583,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B866CB2-420D-49FC-A79A-A6CBDA605C21}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,6 +803,19 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{3AEB1955-C3F3-46B2-92C7-95EFF2A1036A}"/>

</xml_diff>